<commit_message>
Text changes after final reread
</commit_message>
<xml_diff>
--- a/data/cost-of-safety.xlsx
+++ b/data/cost-of-safety.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="-20" windowWidth="33600" windowHeight="20540" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="table&amp;first graph" sheetId="1" r:id="rId1"/>
@@ -948,7 +948,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+    <sheetView topLeftCell="A41" workbookViewId="0">
       <selection activeCell="A70" sqref="A70:E70"/>
     </sheetView>
   </sheetViews>
@@ -2881,19 +2881,19 @@
     </row>
     <row r="58" spans="1:18">
       <c r="A58" s="3">
-        <f t="shared" ref="A58:A70" ca="1" si="19">OFFSET($B$51,0,$R58)</f>
+        <f t="shared" ref="A58:A69" ca="1" si="19">OFFSET($B$51,0,$R58)</f>
         <v>7.8</v>
       </c>
       <c r="B58" s="3">
-        <f t="shared" ref="B58:B70" ca="1" si="20">OFFSET($B$51,1,$R58)</f>
+        <f t="shared" ref="B58:B69" ca="1" si="20">OFFSET($B$51,1,$R58)</f>
         <v>34.694960212201607</v>
       </c>
       <c r="C58" s="3">
-        <f t="shared" ref="C58:C70" ca="1" si="21">OFFSET($B$51,2,$R58)</f>
+        <f t="shared" ref="C58:C69" ca="1" si="21">OFFSET($B$51,2,$R58)</f>
         <v>15.9</v>
       </c>
       <c r="D58" s="3">
-        <f t="shared" ref="D58:D70" ca="1" si="22">OFFSET($B$51,3,$R58)</f>
+        <f t="shared" ref="D58:D69" ca="1" si="22">OFFSET($B$51,3,$R58)</f>
         <v>71.034482758620697</v>
       </c>
       <c r="R58">
@@ -3155,8 +3155,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D42" sqref="A27:D42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35:D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>